<commit_message>
Added links to DOI
</commit_message>
<xml_diff>
--- a/supplementary-table-1.xlsx
+++ b/supplementary-table-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dima\PycharmProjects\gnnom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF6B60A2-2095-43AA-ACD2-7927673A99CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C196E28B-BE3D-4B22-BA35-F0BB0EEF753F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C47A4304-5FC5-451D-BF91-DAAF6AE56D4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C47A4304-5FC5-451D-BF91-DAAF6AE56D4A}"/>
   </bookViews>
   <sheets>
     <sheet name="SASBDB benchmark" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
   <si>
     <t>id</t>
   </si>
@@ -249,7 +249,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,13 +278,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
       <u/>
@@ -327,9 +320,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -337,13 +330,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -663,7 +655,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,6 +667,7 @@
     <col min="8" max="8" width="18.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" style="2"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -706,11 +699,11 @@
       <c r="J1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -744,14 +737,14 @@
         <f t="shared" ref="J2:J10" si="1">ABS(I2-H2)/H2</f>
         <v>3.4502814258911794E-2</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="9">
         <f>AVERAGE(G:G)</f>
         <v>0.10484206505273259</v>
       </c>
-      <c r="N2" s="10">
+      <c r="N2" s="9">
         <f>MEDIAN(G:G)</f>
         <v>7.3190661478599234E-2</v>
       </c>
@@ -763,7 +756,7 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E3" s="1">
@@ -786,14 +779,14 @@
         <f t="shared" si="1"/>
         <v>9.5035026269702227E-2</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="9">
         <f>AVERAGE(J:J)</f>
         <v>7.4191210872138744E-2</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="9">
         <f>MEDIAN(J:J)</f>
         <v>7.6708860759493666E-2</v>
       </c>
@@ -805,10 +798,10 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>479</v>
       </c>
       <c r="F4" s="1">
@@ -836,7 +829,7 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="1">
@@ -867,7 +860,7 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>66</v>
       </c>
       <c r="E6" s="1">
@@ -898,7 +891,7 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E7" s="1">
@@ -929,7 +922,7 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E8" s="1">
@@ -960,7 +953,7 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E9" s="1">
@@ -985,30 +978,30 @@
       </c>
     </row>
     <row r="10" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>66.5</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="11">
         <v>73.356999999999999</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <f t="shared" si="0"/>
         <v>0.10311278195488721</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="11">
         <v>108.976</v>
       </c>
       <c r="J10" s="6"/>
@@ -1020,7 +1013,7 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E11" s="1">
@@ -1051,7 +1044,7 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E12" s="1">
@@ -1113,7 +1106,7 @@
       <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E14" s="1">
@@ -1175,7 +1168,7 @@
       <c r="C16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E16" s="1">
@@ -1206,7 +1199,7 @@
       <c r="C17" t="s">
         <v>35</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E17" s="1">
@@ -1237,7 +1230,7 @@
       <c r="C18" t="s">
         <v>35</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E18" s="1">
@@ -1268,7 +1261,7 @@
       <c r="C19" t="s">
         <v>38</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E19" s="1">
@@ -1454,7 +1447,7 @@
       <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E25" s="1">
@@ -1485,7 +1478,7 @@
       <c r="C26" t="s">
         <v>50</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E26" s="1">
@@ -1543,7 +1536,7 @@
       <c r="C28" t="s">
         <v>54</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E28" s="1">
@@ -1574,7 +1567,7 @@
       <c r="C29" t="s">
         <v>54</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E29" s="1">
@@ -1632,8 +1625,26 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D12" r:id="rId1" display="https://dx.doi.org/10.3390/cryst10110975" xr:uid="{96B6429E-5DC7-41FD-833F-DF03E5E6FD2E}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{E9D2034E-11F0-4117-AFDE-57A7F2A5DFCA}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{CC353623-D18F-4FF3-8E64-54FB27EEBEB9}"/>
+    <hyperlink ref="D11" r:id="rId4" xr:uid="{E00368F8-8B2B-44B0-B5B5-32C69EFA0D94}"/>
+    <hyperlink ref="D14" r:id="rId5" xr:uid="{CEF26C15-7CA1-4F8F-BD29-77D9C75380CB}"/>
+    <hyperlink ref="D28" r:id="rId6" xr:uid="{E577829A-59F2-46B2-87BE-FAEEAFD2F731}"/>
+    <hyperlink ref="D2" r:id="rId7" xr:uid="{09B1E8DA-683C-4181-8C6A-5C48009AFF68}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{BC5492C3-AC28-47B2-9E34-37BFFD648CE5}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{E2A2D3FE-F96B-499E-A2F0-90390F5D0920}"/>
+    <hyperlink ref="D8" r:id="rId10" xr:uid="{12959BCE-FB9D-446C-9149-51EFDB339117}"/>
+    <hyperlink ref="D9" r:id="rId11" xr:uid="{D1A5B720-C10D-4A36-BF15-433A80456CA6}"/>
+    <hyperlink ref="D10" r:id="rId12" xr:uid="{42331C55-73ED-4ABD-8F04-C6EA1C72DEFE}"/>
+    <hyperlink ref="D17" r:id="rId13" xr:uid="{F346D686-03EB-42F4-B287-0EB01A8C1024}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{70E40B87-C718-4BAD-9BD7-6C395F57033E}"/>
+    <hyperlink ref="D25" r:id="rId15" xr:uid="{3089AB40-2A15-4F3D-9094-3B5D241A60AE}"/>
+    <hyperlink ref="D26" r:id="rId16" xr:uid="{B1D6EA78-9E53-452D-B74C-FCA445450FB0}"/>
+    <hyperlink ref="D16" r:id="rId17" xr:uid="{80966459-828B-4673-A4F9-31E62A336F07}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{D8228C83-299F-4AC5-BD01-A6D9999E0818}"/>
+    <hyperlink ref="D29" r:id="rId19" xr:uid="{543366E4-B9BE-42D5-9555-065FA965DFF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Typo: Corrected links to Mylonas.
</commit_message>
<xml_diff>
--- a/supplementary-table-1.xlsx
+++ b/supplementary-table-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dima\PycharmProjects\gnnom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C196E28B-BE3D-4B22-BA35-F0BB0EEF753F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C828A58E-4499-4D8E-8559-DF8A37AB8DCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C47A4304-5FC5-451D-BF91-DAAF6AE56D4A}"/>
   </bookViews>
@@ -655,7 +655,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>